<commit_message>
Signed-off-by: George Dalakos <gdalakos@gmail.com>
</commit_message>
<xml_diff>
--- a/Final_report_supporting_data.xlsx
+++ b/Final_report_supporting_data.xlsx
@@ -1,33 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joanne\Desktop\Festival\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joanne\Desktop\George\festival\FestivalFinanceFramework\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C16973F-2FB9-4D46-891B-C9A37F5C19E1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="270" yWindow="270" windowWidth="10950" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>2016 Festival</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>% Difference</t>
   </si>
@@ -53,37 +56,16 @@
     <t>Festival Profit</t>
   </si>
   <si>
-    <t>2017 Festival</t>
-  </si>
-  <si>
-    <t>Gross =                                       $138,576.20</t>
-  </si>
-  <si>
-    <t>Expenses (Not including Capex) =              $70,537.02</t>
-  </si>
-  <si>
-    <t>Expenses (Not including Capex or inventory) = $69,787.02</t>
-  </si>
-  <si>
-    <t>Expenses (Capex) =                            $6,480.64</t>
-  </si>
-  <si>
-    <t>Profit (Not including Capex) =                $68,039.18</t>
-  </si>
-  <si>
-    <t>Profit (Not including Capex or inventory) =   $68,789.18</t>
-  </si>
-  <si>
-    <t>Profit (Including Capex) =                    $61,558.54</t>
-  </si>
-  <si>
-    <t>Food &amp; beverage sales during festival =       $87,563.56</t>
+    <t>CURRENT YEAR</t>
+  </si>
+  <si>
+    <t>PREVIOUS YEAR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -520,11 +502,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B2:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,160 +517,129 @@
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>0</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="4">
-        <v>25872.28</v>
+        <v>1</v>
       </c>
       <c r="D4" s="5">
-        <v>22181.83</v>
+        <v>1</v>
       </c>
       <c r="E4" s="6">
         <f t="shared" ref="E4:E7" si="0">(C4-D4)/D4</f>
-        <v>0.16637265726046935</v>
-      </c>
-      <c r="H4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="4">
-        <v>44501.11</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5">
-        <v>44201.59</v>
+        <v>1</v>
       </c>
       <c r="E5" s="6">
         <f t="shared" si="0"/>
-        <v>6.7762268280395369E-3</v>
-      </c>
-      <c r="H5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="4">
-        <v>17175.330000000002</v>
+        <v>1</v>
       </c>
       <c r="D6" s="5">
-        <v>14413.3</v>
+        <v>1</v>
       </c>
       <c r="E6" s="6">
         <f t="shared" si="0"/>
-        <v>0.19163064669437274</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="4">
-        <v>87006.83</v>
+        <v>1</v>
       </c>
       <c r="D7" s="5">
-        <v>80796.72</v>
+        <v>1</v>
       </c>
       <c r="E7" s="6">
         <f t="shared" si="0"/>
-        <v>7.6860917126338801E-2</v>
-      </c>
-      <c r="H7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="4">
-        <v>139376.20000000001</v>
+        <v>1</v>
       </c>
       <c r="D8" s="5">
-        <v>128766.98</v>
+        <v>1</v>
       </c>
       <c r="E8" s="6">
         <f>(C8-D8)/D8</f>
-        <v>8.2390842745554929E-2</v>
-      </c>
-      <c r="H8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="4">
-        <v>70479.070000000007</v>
+        <v>1</v>
       </c>
       <c r="D9" s="5">
-        <v>62040.99</v>
+        <v>1</v>
       </c>
       <c r="E9" s="6">
         <f>(C9-D9)/D9</f>
-        <v>0.13600814558246105</v>
-      </c>
-      <c r="H9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="4">
-        <v>68897.13</v>
+        <v>1</v>
       </c>
       <c r="D10" s="5">
-        <v>66725.990000000005</v>
+        <v>1</v>
       </c>
       <c r="E10" s="6">
         <f>(C10-D10)/D10</f>
-        <v>3.2538145930843428E-2</v>
-      </c>
-      <c r="H10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D13" s="7">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D14" s="8">
-        <f>100*D13/14950</f>
-        <v>4.3143812709030103</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D14" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>